<commit_message>
Se genera xlsx, hace falta monat por menores
</commit_message>
<xml_diff>
--- a/Pol_rtas.xlsx
+++ b/Pol_rtas.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Proyecciones" sheetId="1" r:id="rId1"/>
+    <sheet name="Coordenadas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="37">
   <si>
     <t>Δ</t>
   </si>
@@ -37,10 +38,10 @@
     <t>Dist</t>
   </si>
   <si>
-    <t>Proy N</t>
-  </si>
-  <si>
-    <t>Proy E</t>
+    <t>Proy Y</t>
+  </si>
+  <si>
+    <t>Proy X</t>
   </si>
   <si>
     <t>CT21</t>
@@ -113,6 +114,18 @@
   </si>
   <si>
     <t>283° 34'32.0</t>
+  </si>
+  <si>
+    <t>Corr Y</t>
+  </si>
+  <si>
+    <t>Corr X</t>
+  </si>
+  <si>
+    <t>Coord N</t>
+  </si>
+  <si>
+    <t>Coord E</t>
   </si>
 </sst>
 </file>
@@ -740,4 +753,197 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>-40.192</v>
+      </c>
+      <c r="B3">
+        <v>-58.299</v>
+      </c>
+      <c r="C3">
+        <v>0.004</v>
+      </c>
+      <c r="D3">
+        <v>-0.004</v>
+      </c>
+      <c r="E3">
+        <v>1115.933</v>
+      </c>
+      <c r="F3">
+        <v>2161.421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>60.445</v>
+      </c>
+      <c r="B5">
+        <v>-25.621</v>
+      </c>
+      <c r="C5">
+        <v>0.004</v>
+      </c>
+      <c r="D5">
+        <v>-0.004</v>
+      </c>
+      <c r="E5">
+        <v>1075.746</v>
+      </c>
+      <c r="F5">
+        <v>2103.118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>-20.267</v>
+      </c>
+      <c r="B7">
+        <v>83.93300000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.005</v>
+      </c>
+      <c r="D7">
+        <v>-0.005</v>
+      </c>
+      <c r="E7">
+        <v>1136.195</v>
+      </c>
+      <c r="F7">
+        <v>2077.493</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>1115.933</v>
+      </c>
+      <c r="F9">
+        <v>2161.421</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se corrigen algunas cosas de la precision
</commit_message>
<xml_diff>
--- a/Pol_rtas.xlsx
+++ b/Pol_rtas.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Proyecciones" sheetId="1" r:id="rId1"/>
     <sheet name="Coordenadas" sheetId="2" r:id="rId2"/>
+    <sheet name="Parametros Pol" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="53">
   <si>
     <t>Δ</t>
   </si>
@@ -126,6 +127,54 @@
   </si>
   <si>
     <t>Coord E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>ΣOBS</t>
+  </si>
+  <si>
+    <t>ΣTeo</t>
+  </si>
+  <si>
+    <t>e ang</t>
+  </si>
+  <si>
+    <t>e perm</t>
+  </si>
+  <si>
+    <t>corr ang</t>
+  </si>
+  <si>
+    <t>900° 0'20.0</t>
+  </si>
+  <si>
+    <t>900° 0'0.0</t>
+  </si>
+  <si>
+    <t>0° 0'20.0</t>
+  </si>
+  <si>
+    <t>0° 0'10.0</t>
+  </si>
+  <si>
+    <t>ΣDIST</t>
+  </si>
+  <si>
+    <t>ΔPNS</t>
+  </si>
+  <si>
+    <t>ΔPEW</t>
+  </si>
+  <si>
+    <t>e dist</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -946,4 +995,99 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2">
+        <v>222.807</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <v>-0.01407894390836262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>0.01240938702116523</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5">
+        <v>0.01876724667648094</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6">
+        <v>11872.11975421099</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se deja a medias lo de crandall, hace falta verificar suma de proyecciones
</commit_message>
<xml_diff>
--- a/Pol_rtas.xlsx
+++ b/Pol_rtas.xlsx
@@ -45,7 +45,7 @@
     <t>Proy X</t>
   </si>
   <si>
-    <t>CT21</t>
+    <t>CD20</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -57,13 +57,13 @@
     <t>D2</t>
   </si>
   <si>
-    <t>CT20</t>
-  </si>
-  <si>
     <t>D3</t>
   </si>
   <si>
-    <t>C20</t>
+    <t>CD17</t>
+  </si>
+  <si>
+    <t>D4</t>
   </si>
   <si>
     <t>0° 0'0.0</t>
@@ -159,7 +159,7 @@
     <t>0° 0'20.0</t>
   </si>
   <si>
-    <t>0° 0'10.0</t>
+    <t>0° 0'30.0</t>
   </si>
   <si>
     <t>ΣDIST</t>
@@ -572,7 +572,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -717,7 +717,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -860,10 +860,10 @@
         <v>-58.299</v>
       </c>
       <c r="C3">
-        <v>0.004</v>
+        <v>0.005</v>
       </c>
       <c r="D3">
-        <v>-0.004</v>
+        <v>-0.005</v>
       </c>
       <c r="E3">
         <v>1115.933</v>
@@ -900,16 +900,16 @@
         <v>-25.621</v>
       </c>
       <c r="C5">
-        <v>0.004</v>
+        <v>0.007</v>
       </c>
       <c r="D5">
-        <v>-0.004</v>
+        <v>-0.001</v>
       </c>
       <c r="E5">
         <v>1075.746</v>
       </c>
       <c r="F5">
-        <v>2103.118</v>
+        <v>2103.117</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -940,16 +940,16 @@
         <v>83.93300000000001</v>
       </c>
       <c r="C7">
-        <v>0.005</v>
+        <v>0.002</v>
       </c>
       <c r="D7">
-        <v>-0.005</v>
+        <v>-0.007</v>
       </c>
       <c r="E7">
-        <v>1136.195</v>
+        <v>1136.198</v>
       </c>
       <c r="F7">
-        <v>2077.493</v>
+        <v>2077.495</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1042,7 +1042,7 @@
         <v>49</v>
       </c>
       <c r="D3">
-        <v>-0.01407894390836262</v>
+        <v>-0.01399999999999935</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1056,7 +1056,7 @@
         <v>50</v>
       </c>
       <c r="D4">
-        <v>0.01240938702116523</v>
+        <v>0.01300000000000523</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1070,7 +1070,7 @@
         <v>51</v>
       </c>
       <c r="D5">
-        <v>0.01876724667648094</v>
+        <v>0.01910497317454588</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1084,7 +1084,7 @@
         <v>52</v>
       </c>
       <c r="D6">
-        <v>11872.11975421099</v>
+        <v>11662.25139205389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se corrijen los otros dos metodos, hace falta revisar muy bien crandall
</commit_message>
<xml_diff>
--- a/Pol_rtas.xlsx
+++ b/Pol_rtas.xlsx
@@ -860,10 +860,10 @@
         <v>-58.299</v>
       </c>
       <c r="C3">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="D3">
-        <v>-0.005</v>
+        <v>-0.004</v>
       </c>
       <c r="E3">
         <v>1115.933</v>
@@ -900,16 +900,16 @@
         <v>-25.621</v>
       </c>
       <c r="C5">
-        <v>0.007</v>
+        <v>0.005</v>
       </c>
       <c r="D5">
-        <v>-0.001</v>
+        <v>-0.004</v>
       </c>
       <c r="E5">
-        <v>1075.746</v>
+        <v>1075.745</v>
       </c>
       <c r="F5">
-        <v>2103.117</v>
+        <v>2103.118</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -940,16 +940,16 @@
         <v>83.93300000000001</v>
       </c>
       <c r="C7">
-        <v>0.002</v>
+        <v>0.005</v>
       </c>
       <c r="D7">
-        <v>-0.007</v>
+        <v>-0.005</v>
       </c>
       <c r="E7">
-        <v>1136.198</v>
+        <v>1136.195</v>
       </c>
       <c r="F7">
-        <v>2077.495</v>
+        <v>2077.493</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1042,7 +1042,7 @@
         <v>49</v>
       </c>
       <c r="D3">
-        <v>-0.01399999999999935</v>
+        <v>-0.014</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1056,7 +1056,7 @@
         <v>50</v>
       </c>
       <c r="D4">
-        <v>0.01300000000000523</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1070,7 +1070,7 @@
         <v>51</v>
       </c>
       <c r="D5">
-        <v>0.01910497317454588</v>
+        <v>0.0191049731745428</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1084,7 +1084,7 @@
         <v>52</v>
       </c>
       <c r="D6">
-        <v>11662.25139205389</v>
+        <v>11662.25139205577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se saca metodo de crandall es solo acomodar excel y pasarlo a txt, fiesta en america
</commit_message>
<xml_diff>
--- a/Pol_rtas.xlsx
+++ b/Pol_rtas.xlsx
@@ -860,10 +860,10 @@
         <v>-58.299</v>
       </c>
       <c r="C3">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="D3">
-        <v>-0.004</v>
+        <v>0.003</v>
       </c>
       <c r="E3">
         <v>1115.933</v>
@@ -900,16 +900,16 @@
         <v>-25.621</v>
       </c>
       <c r="C5">
-        <v>0.005</v>
+        <v>0.013</v>
       </c>
       <c r="D5">
-        <v>-0.004</v>
+        <v>-0.005</v>
       </c>
       <c r="E5">
         <v>1075.745</v>
       </c>
       <c r="F5">
-        <v>2103.118</v>
+        <v>2103.124</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -940,16 +940,16 @@
         <v>83.93300000000001</v>
       </c>
       <c r="C7">
-        <v>0.005</v>
+        <v>0.002</v>
       </c>
       <c r="D7">
-        <v>-0.005</v>
+        <v>-0.01</v>
       </c>
       <c r="E7">
-        <v>1136.195</v>
+        <v>1136.204</v>
       </c>
       <c r="F7">
-        <v>2077.493</v>
+        <v>2077.501</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -989,7 +989,7 @@
         <v>1115.933</v>
       </c>
       <c r="F9">
-        <v>2161.421</v>
+        <v>2161.422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se realiza todo lo de la poligonal
</commit_message>
<xml_diff>
--- a/Pol_rtas.xlsx
+++ b/Pol_rtas.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoda\Desktop\Materias U\Materias 5 semestre\Ing de software\proyecto_ing_software\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05076AA0-DAF7-4765-BB1B-1070D48E30AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1392" yWindow="1740" windowWidth="19152" windowHeight="10764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proyecciones" sheetId="1" r:id="rId1"/>
     <sheet name="Coordenadas" sheetId="2" r:id="rId2"/>
     <sheet name="Parametros Pol" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="55">
   <si>
     <t>Δ</t>
   </si>
@@ -121,6 +127,12 @@
   </si>
   <si>
     <t>Corr X</t>
+  </si>
+  <si>
+    <t>Proy corr Y</t>
+  </si>
+  <si>
+    <t>Proy corr X</t>
   </si>
   <si>
     <t>Coord N</t>
@@ -180,8 +192,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,11 +256,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -290,7 +310,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,9 +342,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -356,6 +394,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -531,14 +587,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,7 +623,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -596,7 +652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -616,16 +672,16 @@
         <v>27</v>
       </c>
       <c r="G3">
-        <v>70.81100000000001</v>
+        <v>70.811000000000007</v>
       </c>
       <c r="H3">
         <v>-40.192</v>
       </c>
       <c r="I3">
-        <v>-58.299</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>-58.298999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -654,7 +710,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -674,16 +730,16 @@
         <v>29</v>
       </c>
       <c r="G5">
-        <v>65.651</v>
+        <v>65.650999999999996</v>
       </c>
       <c r="H5">
         <v>60.445</v>
       </c>
       <c r="I5">
-        <v>-25.621</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>-25.620999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -712,7 +768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -732,16 +788,16 @@
         <v>31</v>
       </c>
       <c r="G7">
-        <v>86.345</v>
+        <v>86.344999999999999</v>
       </c>
       <c r="H7">
-        <v>-20.267</v>
+        <v>-20.266999999999999</v>
       </c>
       <c r="I7">
-        <v>83.93300000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>83.933000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -770,7 +826,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -805,14 +861,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -831,8 +889,14 @@
       <c r="F1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -851,28 +915,40 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>-40.192</v>
       </c>
       <c r="B3">
-        <v>-58.299</v>
+        <v>-58.298999999999999</v>
       </c>
       <c r="C3">
-        <v>0.002</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3">
-        <v>0.003</v>
+        <v>-5.0000000000000001E-3</v>
       </c>
       <c r="E3">
+        <v>-40.186999999999998</v>
+      </c>
+      <c r="F3">
+        <v>-58.304000000000002</v>
+      </c>
+      <c r="G3">
         <v>1115.933</v>
       </c>
-      <c r="F3">
-        <v>2161.421</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3">
+        <v>2161.4209999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -891,28 +967,40 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>60.445</v>
       </c>
       <c r="B5">
-        <v>-25.621</v>
+        <v>-25.620999999999999</v>
       </c>
       <c r="C5">
-        <v>0.013</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D5">
-        <v>-0.005</v>
+        <v>-1E-3</v>
       </c>
       <c r="E5">
-        <v>1075.745</v>
+        <v>60.451999999999998</v>
       </c>
       <c r="F5">
-        <v>2103.124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>-25.622</v>
+      </c>
+      <c r="G5">
+        <v>1075.7460000000001</v>
+      </c>
+      <c r="H5">
+        <v>2103.1170000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -931,28 +1019,40 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>-20.267</v>
+        <v>-20.266999999999999</v>
       </c>
       <c r="B7">
-        <v>83.93300000000001</v>
+        <v>83.933000000000007</v>
       </c>
       <c r="C7">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="D7">
-        <v>-0.01</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="E7">
-        <v>1136.204</v>
+        <v>-20.265000000000001</v>
       </c>
       <c r="F7">
-        <v>2077.501</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>83.926000000000002</v>
+      </c>
+      <c r="G7">
+        <v>1136.1980000000001</v>
+      </c>
+      <c r="H7">
+        <v>2077.4949999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -971,8 +1071,14 @@
       <c r="F8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -985,11 +1091,17 @@
       <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9">
         <v>1115.933</v>
       </c>
-      <c r="F9">
-        <v>2161.422</v>
+      <c r="H9">
+        <v>2161.4209999999998</v>
       </c>
     </row>
   </sheetData>
@@ -998,90 +1110,92 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="A4:E18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>222.80699999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3">
+        <v>-1.4E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2">
-        <v>222.807</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5">
+        <v>1.9104973174542801E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3">
-        <v>-0.014</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5">
-        <v>0.0191049731745428</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D6">
         <v>11662.25139205577</v>

</xml_diff>

<commit_message>
Se corrige la parte angular
</commit_message>
<xml_diff>
--- a/Pol_rtas.xlsx
+++ b/Pol_rtas.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leoda\Desktop\Materias U\Materias 5 semestre\Ing de software\proyecto_ing_software\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05076AA0-DAF7-4765-BB1B-1070D48E30AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1392" yWindow="1740" windowWidth="19152" windowHeight="10764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Proyecciones" sheetId="1" r:id="rId1"/>
     <sheet name="Coordenadas" sheetId="2" r:id="rId2"/>
     <sheet name="Parametros Pol" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="58">
   <si>
     <t>Δ</t>
   </si>
@@ -51,76 +45,85 @@
     <t>Proy X</t>
   </si>
   <si>
-    <t>CD20</t>
+    <t>V6</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>D1</t>
+    <t>C#5</t>
   </si>
   <si>
     <t>D2</t>
   </si>
   <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>CD17</t>
-  </si>
-  <si>
-    <t>D4</t>
+    <t>IS-2</t>
+  </si>
+  <si>
+    <t>PR</t>
   </si>
   <si>
     <t>0° 0'0.0</t>
   </si>
   <si>
-    <t>236° 45'56.0</t>
-  </si>
-  <si>
-    <t>281° 36'48.0</t>
-  </si>
-  <si>
-    <t>306° 32'51.0</t>
-  </si>
-  <si>
-    <t>75° 4'45.0</t>
-  </si>
-  <si>
-    <t>-0° 0'5.0</t>
-  </si>
-  <si>
-    <t>236° 45'51.0</t>
-  </si>
-  <si>
-    <t>281° 36'43.0</t>
-  </si>
-  <si>
-    <t>306° 32'46.0</t>
-  </si>
-  <si>
-    <t>75° 4'40.0</t>
+    <t>63° 31'6.0</t>
+  </si>
+  <si>
+    <t>272° 20'40.0</t>
+  </si>
+  <si>
+    <t>250° 26'20.0</t>
+  </si>
+  <si>
+    <t>224° 54'0.0</t>
+  </si>
+  <si>
+    <t>268° 47'46.0</t>
+  </si>
+  <si>
+    <t>0° 0'2.0</t>
+  </si>
+  <si>
+    <t>63° 31'8.0</t>
+  </si>
+  <si>
+    <t>272° 20'42.0</t>
+  </si>
+  <si>
+    <t>250° 26'22.0</t>
+  </si>
+  <si>
+    <t>224° 54'2.0</t>
+  </si>
+  <si>
+    <t>268° 47'48.0</t>
   </si>
   <si>
     <t>358° 39'12.0</t>
   </si>
   <si>
-    <t>235° 25'3.0</t>
-  </si>
-  <si>
-    <t>55° 25'3.0</t>
-  </si>
-  <si>
-    <t>337° 1'46.0</t>
-  </si>
-  <si>
-    <t>157° 1'46.0</t>
-  </si>
-  <si>
-    <t>103° 34'32.0</t>
-  </si>
-  <si>
-    <t>283° 34'32.0</t>
+    <t>62° 10'19.0</t>
+  </si>
+  <si>
+    <t>242° 10'19.0</t>
+  </si>
+  <si>
+    <t>154° 31'1.0</t>
+  </si>
+  <si>
+    <t>334° 31'1.0</t>
+  </si>
+  <si>
+    <t>224° 57'22.0</t>
+  </si>
+  <si>
+    <t>44° 57'22.0</t>
+  </si>
+  <si>
+    <t>269° 51'24.0</t>
+  </si>
+  <si>
+    <t>89° 51'24.0</t>
   </si>
   <si>
     <t>Corr Y</t>
@@ -162,16 +165,16 @@
     <t>corr ang</t>
   </si>
   <si>
-    <t>900° 0'20.0</t>
-  </si>
-  <si>
-    <t>900° 0'0.0</t>
-  </si>
-  <si>
-    <t>0° 0'20.0</t>
-  </si>
-  <si>
-    <t>0° 0'30.0</t>
+    <t>1079° 59'52.0</t>
+  </si>
+  <si>
+    <t>1080° 0'0.0</t>
+  </si>
+  <si>
+    <t>-0° 0'8.0</t>
+  </si>
+  <si>
+    <t>0° 0'40.0</t>
   </si>
   <si>
     <t>ΣDIST</t>
@@ -192,8 +195,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,19 +259,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -310,7 +305,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,27 +337,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -394,24 +371,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -587,14 +546,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +582,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -631,7 +590,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -640,7 +599,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -652,7 +611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -660,7 +619,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
@@ -669,19 +628,19 @@
         <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3">
-        <v>70.811000000000007</v>
+        <v>46.141</v>
       </c>
       <c r="H3">
-        <v>-40.192</v>
+        <v>21.539</v>
       </c>
       <c r="I3">
-        <v>-58.298999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40.805</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -689,7 +648,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -698,7 +657,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -710,7 +669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -718,7 +677,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -727,19 +686,19 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G5">
-        <v>65.650999999999996</v>
+        <v>10.077</v>
       </c>
       <c r="H5">
-        <v>60.445</v>
+        <v>-9.097</v>
       </c>
       <c r="I5">
-        <v>-25.620999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -747,7 +706,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -756,7 +715,7 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
@@ -768,7 +727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -776,7 +735,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -785,19 +744,19 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G7">
-        <v>86.344999999999999</v>
+        <v>17.637</v>
       </c>
       <c r="H7">
-        <v>-20.266999999999999</v>
+        <v>-12.481</v>
       </c>
       <c r="I7">
-        <v>83.933000000000007</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>-12.462</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -805,7 +764,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -814,7 +773,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
         <v>10</v>
@@ -826,15 +785,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
@@ -843,15 +802,73 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9">
+        <v>32.736</v>
+      </c>
+      <c r="H9">
+        <v>-0.082</v>
+      </c>
+      <c r="I9">
+        <v>-32.736</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
         <v>26</v>
       </c>
-      <c r="G9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -861,16 +878,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -878,25 +893,25 @@
         <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -922,33 +937,33 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3">
-        <v>-40.192</v>
+        <v>21.539</v>
       </c>
       <c r="B3">
-        <v>-58.298999999999999</v>
+        <v>40.805</v>
       </c>
       <c r="C3">
-        <v>5.0000000000000001E-3</v>
+        <v>0.052</v>
       </c>
       <c r="D3">
-        <v>-5.0000000000000001E-3</v>
+        <v>0.025</v>
       </c>
       <c r="E3">
-        <v>-40.186999999999998</v>
+        <v>21.591</v>
       </c>
       <c r="F3">
-        <v>-58.304000000000002</v>
+        <v>40.83</v>
       </c>
       <c r="G3">
         <v>1115.933</v>
       </c>
       <c r="H3">
-        <v>2161.4209999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2161.421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -974,33 +989,33 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5">
-        <v>60.445</v>
+        <v>-9.097</v>
       </c>
       <c r="B5">
-        <v>-25.620999999999999</v>
+        <v>4.336</v>
       </c>
       <c r="C5">
-        <v>7.0000000000000001E-3</v>
+        <v>0.012</v>
       </c>
       <c r="D5">
-        <v>-1E-3</v>
+        <v>0.005</v>
       </c>
       <c r="E5">
-        <v>60.451999999999998</v>
+        <v>-9.084999999999999</v>
       </c>
       <c r="F5">
-        <v>-25.622</v>
+        <v>4.341</v>
       </c>
       <c r="G5">
-        <v>1075.7460000000001</v>
+        <v>1137.524</v>
       </c>
       <c r="H5">
-        <v>2103.1170000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2202.251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1026,33 +1041,33 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7">
-        <v>-20.266999999999999</v>
+        <v>-12.481</v>
       </c>
       <c r="B7">
-        <v>83.933000000000007</v>
+        <v>-12.462</v>
       </c>
       <c r="C7">
-        <v>2E-3</v>
+        <v>0.02</v>
       </c>
       <c r="D7">
-        <v>-7.0000000000000001E-3</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E7">
-        <v>-20.265000000000001</v>
+        <v>-12.461</v>
       </c>
       <c r="F7">
-        <v>83.926000000000002</v>
+        <v>-12.453</v>
       </c>
       <c r="G7">
-        <v>1136.1980000000001</v>
+        <v>1128.439</v>
       </c>
       <c r="H7">
-        <v>2077.4949999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2206.592</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1078,30 +1093,82 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>-0.082</v>
+      </c>
+      <c r="B9">
+        <v>-32.736</v>
+      </c>
+      <c r="C9">
+        <v>0.037</v>
+      </c>
+      <c r="D9">
+        <v>0.018</v>
+      </c>
+      <c r="E9">
+        <v>-0.04500000000000001</v>
+      </c>
+      <c r="F9">
+        <v>-32.718</v>
       </c>
       <c r="G9">
+        <v>1115.978</v>
+      </c>
+      <c r="H9">
+        <v>2194.139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11">
         <v>1115.933</v>
       </c>
-      <c r="H9">
-        <v>2161.4209999999998</v>
+      <c r="H11">
+        <v>2161.421</v>
       </c>
     </row>
   </sheetData>
@@ -1110,95 +1177,93 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="A4:E18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2">
+        <v>106.591</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3">
+        <v>-0.121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>46</v>
       </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2">
-        <v>222.80699999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4">
+        <v>-0.057</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>47</v>
       </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3">
-        <v>-1.4E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>0.1337535046269817</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4">
-        <v>1.2999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5">
-        <v>1.9104973174542801E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>45</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D6">
-        <v>11662.25139205577</v>
+        <v>796.9211744938287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>